<commit_message>
Update lab 7 xlsx file
</commit_message>
<xml_diff>
--- a/Data_Sets/Lab-7-carbon-dioxide-concentrations.xlsx
+++ b/Data_Sets/Lab-7-carbon-dioxide-concentrations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beebee/Documents/GitHub/Intro-Stats-Excel-Lab-Manual/Data_Sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74589DF5-7051-AA48-B2DB-8D442BB06BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC24BFA1-3F04-5348-96D6-6DDCF4E4A1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,7 +902,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>